<commit_message>
feature by feature eda. implemented get model data function.
</commit_message>
<xml_diff>
--- a/Supplemental_Excel.xlsx
+++ b/Supplemental_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\OneDrive\Desktop\ReposGoHere\PublicRepos\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="8_{5C73338D-B8EC-4B18-9CAD-7B9B9CA15394}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{994815B0-338D-44D3-B3D3-7A00342BCEE9}"/>
+  <xr:revisionPtr revIDLastSave="369" documentId="8_{5C73338D-B8EC-4B18-9CAD-7B9B9CA15394}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{416908B1-A18E-4845-A13A-43679C088098}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" activeTab="1" xr2:uid="{261272EC-EE60-44CA-9508-88C02FE8EAF8}"/>
   </bookViews>
@@ -6353,7 +6353,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 52983"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -7535,13 +7535,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1265238</xdr:colOff>
+      <xdr:colOff>1264445</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>296863</xdr:colOff>
+      <xdr:colOff>296070</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>130175</xdr:rowOff>
     </xdr:to>
@@ -7558,8 +7558,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1265238" y="5753100"/>
-          <a:ext cx="1308100" cy="539750"/>
+          <a:off x="1264445" y="5721350"/>
+          <a:ext cx="1317625" cy="536575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7610,13 +7610,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1019176</xdr:colOff>
+      <xdr:colOff>1018382</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>130175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>542926</xdr:colOff>
+      <xdr:colOff>542132</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -7633,8 +7633,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1019176" y="6835775"/>
-          <a:ext cx="1800225" cy="736600"/>
+          <a:off x="1018382" y="6797675"/>
+          <a:ext cx="1809750" cy="732367"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -7685,13 +7685,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1266826</xdr:colOff>
+      <xdr:colOff>1266032</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>53975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>295276</xdr:colOff>
+      <xdr:colOff>294482</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -7708,8 +7708,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1266826" y="8207375"/>
-          <a:ext cx="1304925" cy="555625"/>
+          <a:off x="1266032" y="8160808"/>
+          <a:ext cx="1314450" cy="552450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7760,13 +7760,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1020763</xdr:colOff>
+      <xdr:colOff>1019970</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>541338</xdr:colOff>
+      <xdr:colOff>540545</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
@@ -7783,8 +7783,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1020763" y="9420225"/>
-          <a:ext cx="1797050" cy="730250"/>
+          <a:off x="1019970" y="9366250"/>
+          <a:ext cx="1806575" cy="726017"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -7835,13 +7835,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1017588</xdr:colOff>
+      <xdr:colOff>1016795</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>544513</xdr:colOff>
+      <xdr:colOff>543720</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -7858,8 +7858,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1017588" y="10801350"/>
-          <a:ext cx="1803400" cy="733425"/>
+          <a:off x="1016795" y="10739967"/>
+          <a:ext cx="1812925" cy="729191"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -7910,15 +7910,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1016001</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>1018382</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>539751</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:colOff>542132</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>98426</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7933,8 +7933,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1016001" y="12160250"/>
-          <a:ext cx="1800225" cy="733425"/>
+          <a:off x="1018382" y="13413317"/>
+          <a:ext cx="1809750" cy="729192"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -7985,13 +7985,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>249239</xdr:colOff>
+      <xdr:colOff>251090</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>130175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
+      <xdr:colOff>251091</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>130175</xdr:rowOff>
     </xdr:to>
@@ -8011,8 +8011,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1916114" y="6292850"/>
-          <a:ext cx="3174" cy="542925"/>
+          <a:off x="1923257" y="6257925"/>
+          <a:ext cx="1" cy="539750"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8041,13 +8041,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>249239</xdr:colOff>
+      <xdr:colOff>251090</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>249239</xdr:colOff>
+      <xdr:colOff>251090</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
@@ -8067,8 +8067,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1916114" y="7569200"/>
-          <a:ext cx="0" cy="638175"/>
+          <a:off x="1923257" y="7530042"/>
+          <a:ext cx="0" cy="630766"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8097,13 +8097,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>249239</xdr:colOff>
+      <xdr:colOff>251090</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
+      <xdr:colOff>251091</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -8123,8 +8123,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1916114" y="8759825"/>
-          <a:ext cx="3174" cy="660400"/>
+          <a:off x="1923257" y="8713258"/>
+          <a:ext cx="1" cy="652992"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8153,22 +8153,340 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
+      <xdr:colOff>251091</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251091</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="122" name="Straight Arrow Connector 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F6BA718-26CF-4946-93B3-72966F7F1969}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="103" idx="4"/>
+          <a:endCxn id="109" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1923258" y="11469158"/>
+          <a:ext cx="0" cy="680509"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1264445</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>32809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>296070</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>45509</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="125" name="Rectangle 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD21E385-7EF7-4E2D-8159-1BF611C9405E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1264445" y="14796559"/>
+          <a:ext cx="1317625" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>predictive model</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251090</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>98426</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251091</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>32809</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="126" name="Straight Arrow Connector 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BEC402F-7058-48A3-A693-278D9FAED001}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="104" idx="4"/>
+          <a:endCxn id="125" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1923257" y="14142509"/>
+          <a:ext cx="1" cy="654050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1266562</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293953</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>91017</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="Rectangle 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B39C02AB-04F0-414D-B3F7-5ECD00E0E9A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266562" y="12149667"/>
+          <a:ext cx="1313391" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>data_engineered</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251090</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>91017</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251091</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="114" name="Straight Arrow Connector 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{636FF6CB-6CB2-4D5F-A2AC-36EACE5A0B0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="109" idx="2"/>
+          <a:endCxn id="104" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1923257" y="12695767"/>
+          <a:ext cx="1" cy="717550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251091</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
+      <xdr:colOff>251091</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="121" name="Straight Arrow Connector 120">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FBCAF61-14F6-4168-9AD7-9A43B48E344D}"/>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59F1698C-2382-45CF-B3B8-5203EFAE14C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8179,211 +8497,25 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1919288" y="10153650"/>
+          <a:off x="1923258" y="10092267"/>
           <a:ext cx="0" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
+        <a:lnRef idx="2">
           <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
           <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>252414</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="122" name="Straight Arrow Connector 121">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F6BA718-26CF-4946-93B3-72966F7F1969}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="103" idx="4"/>
-          <a:endCxn id="104" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1919288" y="11531600"/>
-          <a:ext cx="1" cy="631825"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1262063</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>293688</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="125" name="Rectangle 124">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD21E385-7EF7-4E2D-8159-1BF611C9405E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1262063" y="13550900"/>
-          <a:ext cx="1308100" cy="555625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>predictive model</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>252414</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="126" name="Straight Arrow Connector 125">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BEC402F-7058-48A3-A693-278D9FAED001}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="104" idx="4"/>
-          <a:endCxn id="125" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1919288" y="12893675"/>
-          <a:ext cx="1" cy="657225"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -11450,8 +11582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA93D87-C1D9-4C02-9C75-3797DDA0A849}">
   <dimension ref="A1:BN95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>